<commit_message>
Version 0.2.0; build on push to main cdfb7a7b442737dc280d1df000587d76cb33d8e0
</commit_message>
<xml_diff>
--- a/currentbuild/CodeSystem-IplosCs.xlsx
+++ b/currentbuild/CodeSystem-IplosCs.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-12T13:47:08+00:00</t>
+    <t>2025-11-12T16:10:30+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>